<commit_message>
Connected Database To MongoDB Atlas Using Mongoose
</commit_message>
<xml_diff>
--- a/python/List Tugas Gabunggan.xlsx
+++ b/python/List Tugas Gabunggan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\Web Dev Related Stuff\Web Dev\Web Laporan V.3\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A26C29A-7EAB-4BA5-BD9B-E4BE918C7943}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E66180-6EF1-4F04-BB84-638E13526E31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5112" yWindow="2652" windowWidth="10584" windowHeight="8328" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12456" yWindow="1848" windowWidth="10584" windowHeight="8328" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2355" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2429" uniqueCount="159">
   <si>
     <t>No.</t>
   </si>
@@ -493,6 +493,18 @@
   </si>
   <si>
     <t>PKN6</t>
+  </si>
+  <si>
+    <t>Minggu Ke-17</t>
+  </si>
+  <si>
+    <t>BINDO12</t>
+  </si>
+  <si>
+    <t>BINDO13</t>
+  </si>
+  <si>
+    <t>BING9</t>
   </si>
 </sst>
 </file>
@@ -614,7 +626,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -669,25 +681,14 @@
       </left>
       <right/>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -762,7 +763,34 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -771,46 +799,10 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1119,13 +1111,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CC45"/>
+  <dimension ref="A1:CF45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="BX4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="BX8" sqref="BX8:CC8"/>
+      <selection pane="bottomRight" activeCell="BX10" sqref="BX10:CF10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1173,190 +1165,197 @@
     <col min="75" max="75" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="76" max="76" width="9.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="77" max="78" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="9.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="80" max="16384" width="8.88671875" style="1"/>
+    <col min="79" max="81" width="9.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="82" max="83" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="9.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="85" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:81" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:84" ht="18" x14ac:dyDescent="0.3">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="39" t="s">
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="40" t="s">
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="Q1" s="40"/>
-      <c r="R1" s="40"/>
-      <c r="S1" s="40"/>
-      <c r="T1" s="40"/>
-      <c r="U1" s="40"/>
-      <c r="V1" s="40"/>
-      <c r="W1" s="42" t="s">
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="32"/>
+      <c r="U1" s="32"/>
+      <c r="V1" s="32"/>
+      <c r="W1" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="X1" s="42"/>
-      <c r="Y1" s="42"/>
-      <c r="Z1" s="41" t="s">
+      <c r="X1" s="31"/>
+      <c r="Y1" s="31"/>
+      <c r="Z1" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="AA1" s="41"/>
-      <c r="AB1" s="41"/>
-      <c r="AC1" s="41"/>
-      <c r="AD1" s="41"/>
-      <c r="AE1" s="41"/>
-      <c r="AF1" s="41"/>
-      <c r="AG1" s="41"/>
-      <c r="AH1" s="39" t="s">
+      <c r="AA1" s="36"/>
+      <c r="AB1" s="36"/>
+      <c r="AC1" s="36"/>
+      <c r="AD1" s="36"/>
+      <c r="AE1" s="36"/>
+      <c r="AF1" s="36"/>
+      <c r="AG1" s="36"/>
+      <c r="AH1" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="AI1" s="39"/>
-      <c r="AJ1" s="39"/>
-      <c r="AK1" s="39"/>
-      <c r="AL1" s="39"/>
-      <c r="AM1" s="40" t="s">
+      <c r="AI1" s="37"/>
+      <c r="AJ1" s="37"/>
+      <c r="AK1" s="37"/>
+      <c r="AL1" s="37"/>
+      <c r="AM1" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="AN1" s="40"/>
-      <c r="AO1" s="40"/>
-      <c r="AP1" s="42" t="s">
+      <c r="AN1" s="32"/>
+      <c r="AO1" s="32"/>
+      <c r="AP1" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="AQ1" s="42"/>
-      <c r="AR1" s="42"/>
-      <c r="AS1" s="42"/>
-      <c r="AT1" s="42"/>
-      <c r="AU1" s="41" t="s">
+      <c r="AQ1" s="31"/>
+      <c r="AR1" s="31"/>
+      <c r="AS1" s="31"/>
+      <c r="AT1" s="31"/>
+      <c r="AU1" s="36" t="s">
         <v>114</v>
       </c>
-      <c r="AV1" s="41"/>
-      <c r="AW1" s="41"/>
-      <c r="AX1" s="41"/>
-      <c r="AY1" s="41"/>
-      <c r="AZ1" s="41"/>
-      <c r="BA1" s="39" t="s">
+      <c r="AV1" s="36"/>
+      <c r="AW1" s="36"/>
+      <c r="AX1" s="36"/>
+      <c r="AY1" s="36"/>
+      <c r="AZ1" s="36"/>
+      <c r="BA1" s="37" t="s">
         <v>120</v>
       </c>
-      <c r="BB1" s="39"/>
-      <c r="BC1" s="39"/>
-      <c r="BD1" s="39"/>
-      <c r="BE1" s="39"/>
-      <c r="BF1" s="39"/>
-      <c r="BG1" s="40" t="s">
+      <c r="BB1" s="37"/>
+      <c r="BC1" s="37"/>
+      <c r="BD1" s="37"/>
+      <c r="BE1" s="37"/>
+      <c r="BF1" s="37"/>
+      <c r="BG1" s="32" t="s">
         <v>126</v>
       </c>
-      <c r="BH1" s="40"/>
-      <c r="BI1" s="40"/>
-      <c r="BJ1" s="40"/>
+      <c r="BH1" s="32"/>
+      <c r="BI1" s="32"/>
+      <c r="BJ1" s="32"/>
       <c r="BK1" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="BL1" s="41" t="s">
+      <c r="BL1" s="36" t="s">
         <v>134</v>
       </c>
-      <c r="BM1" s="41"/>
-      <c r="BN1" s="41"/>
-      <c r="BO1" s="39" t="s">
+      <c r="BM1" s="36"/>
+      <c r="BN1" s="36"/>
+      <c r="BO1" s="37" t="s">
         <v>138</v>
       </c>
-      <c r="BP1" s="39"/>
-      <c r="BQ1" s="39"/>
-      <c r="BR1" s="39"/>
-      <c r="BS1" s="40" t="s">
+      <c r="BP1" s="37"/>
+      <c r="BQ1" s="37"/>
+      <c r="BR1" s="37"/>
+      <c r="BS1" s="32" t="s">
         <v>146</v>
       </c>
-      <c r="BT1" s="40"/>
-      <c r="BU1" s="40"/>
-      <c r="BV1" s="40"/>
-      <c r="BW1" s="40"/>
-      <c r="BX1" s="34" t="s">
+      <c r="BT1" s="32"/>
+      <c r="BU1" s="32"/>
+      <c r="BV1" s="32"/>
+      <c r="BW1" s="32"/>
+      <c r="BX1" s="31" t="s">
         <v>148</v>
       </c>
-      <c r="BY1" s="35"/>
-      <c r="BZ1" s="35"/>
-      <c r="CA1" s="35"/>
-      <c r="CB1" s="35"/>
-      <c r="CC1" s="35"/>
+      <c r="BY1" s="31"/>
+      <c r="BZ1" s="31"/>
+      <c r="CA1" s="31"/>
+      <c r="CB1" s="31"/>
+      <c r="CC1" s="31"/>
+      <c r="CD1" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="CE1" s="34"/>
+      <c r="CF1" s="34"/>
     </row>
-    <row r="2" spans="1:81" ht="18" x14ac:dyDescent="0.3">
-      <c r="A2" s="38"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="27" t="s">
+    <row r="2" spans="1:84" ht="18" x14ac:dyDescent="0.3">
+      <c r="A2" s="35"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="G2" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="H2" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="28" t="s">
+      <c r="I2" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="28" t="s">
+      <c r="J2" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="28" t="s">
+      <c r="K2" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="28" t="s">
+      <c r="L2" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="28" t="s">
+      <c r="M2" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="N2" s="28" t="s">
+      <c r="N2" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="O2" s="28" t="s">
+      <c r="O2" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="P2" s="26" t="s">
+      <c r="P2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="Q2" s="26" t="s">
+      <c r="Q2" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="R2" s="26" t="s">
+      <c r="R2" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="S2" s="26" t="s">
+      <c r="S2" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="T2" s="26" t="s">
+      <c r="T2" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="U2" s="26" t="s">
+      <c r="U2" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="V2" s="26" t="s">
+      <c r="V2" s="28" t="s">
         <v>48</v>
       </c>
       <c r="W2" s="29" t="s">
@@ -1368,52 +1367,52 @@
       <c r="Y2" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="Z2" s="27" t="s">
+      <c r="Z2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="AA2" s="27" t="s">
+      <c r="AA2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="AB2" s="27" t="s">
+      <c r="AB2" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="AC2" s="27" t="s">
+      <c r="AC2" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="AD2" s="27" t="s">
+      <c r="AD2" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="AE2" s="27" t="s">
+      <c r="AE2" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="AF2" s="27" t="s">
+      <c r="AF2" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="AG2" s="27" t="s">
+      <c r="AG2" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="AH2" s="28" t="s">
+      <c r="AH2" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="AI2" s="28" t="s">
+      <c r="AI2" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="AJ2" s="28" t="s">
+      <c r="AJ2" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="AK2" s="28" t="s">
+      <c r="AK2" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="AL2" s="28" t="s">
+      <c r="AL2" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="AM2" s="26" t="s">
+      <c r="AM2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="AN2" s="26" t="s">
+      <c r="AN2" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="AO2" s="26" t="s">
+      <c r="AO2" s="28" t="s">
         <v>4</v>
       </c>
       <c r="AP2" s="29" t="s">
@@ -1431,115 +1430,124 @@
       <c r="AT2" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="AU2" s="27" t="s">
+      <c r="AU2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="AV2" s="27" t="s">
+      <c r="AV2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="AW2" s="27" t="s">
+      <c r="AW2" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="AX2" s="27" t="s">
+      <c r="AX2" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="AY2" s="27" t="s">
+      <c r="AY2" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="AZ2" s="27" t="s">
+      <c r="AZ2" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="BA2" s="28" t="s">
+      <c r="BA2" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="BB2" s="28" t="s">
+      <c r="BB2" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="BC2" s="28" t="s">
+      <c r="BC2" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="BD2" s="28" t="s">
+      <c r="BD2" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="BE2" s="28" t="s">
+      <c r="BE2" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="BF2" s="28" t="s">
+      <c r="BF2" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="BG2" s="26" t="s">
+      <c r="BG2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="BH2" s="26" t="s">
+      <c r="BH2" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="BI2" s="26" t="s">
+      <c r="BI2" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="BJ2" s="26" t="s">
+      <c r="BJ2" s="28" t="s">
         <v>5</v>
       </c>
       <c r="BK2" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="BL2" s="27" t="s">
+      <c r="BL2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="BM2" s="27" t="s">
+      <c r="BM2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="BN2" s="27" t="s">
+      <c r="BN2" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="BO2" s="28" t="s">
+      <c r="BO2" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="BP2" s="28" t="s">
+      <c r="BP2" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="BQ2" s="28" t="s">
+      <c r="BQ2" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="BR2" s="28" t="s">
+      <c r="BR2" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="BS2" s="26" t="s">
+      <c r="BS2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="BT2" s="26" t="s">
+      <c r="BT2" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="BU2" s="26" t="s">
+      <c r="BU2" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="BV2" s="26" t="s">
+      <c r="BV2" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="BW2" s="26" t="s">
+      <c r="BW2" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="BX2" s="30" t="s">
+      <c r="BX2" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="BY2" s="31" t="s">
+      <c r="BY2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="BZ2" s="31" t="s">
+      <c r="BZ2" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="CA2" s="32" t="s">
+      <c r="CA2" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="CB2" s="33" t="s">
+      <c r="CB2" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="CC2" s="33" t="s">
+      <c r="CC2" s="29" t="s">
         <v>47</v>
       </c>
+      <c r="CD2" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="CE2" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="CF2" s="30" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:81" ht="18" x14ac:dyDescent="0.3">
-      <c r="A3" s="38"/>
-      <c r="B3" s="38"/>
+    <row r="3" spans="1:84" ht="18" x14ac:dyDescent="0.3">
+      <c r="A3" s="35"/>
+      <c r="B3" s="35"/>
       <c r="C3" s="13" t="s">
         <v>58</v>
       </c>
@@ -1777,8 +1785,17 @@
       <c r="CC3" s="3" t="s">
         <v>154</v>
       </c>
+      <c r="CD3" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="CE3" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="CF3" s="13" t="s">
+        <v>158</v>
+      </c>
     </row>
-    <row r="4" spans="1:81" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -1996,22 +2013,39 @@
       <c r="BU4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="BV4" s="22"/>
+      <c r="BV4" s="8" t="s">
+        <v>12</v>
+      </c>
       <c r="BW4" s="7" t="s">
         <v>12</v>
       </c>
       <c r="BX4" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="BY4" s="5"/>
-      <c r="BZ4" s="23"/>
+      <c r="BY4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="BZ4" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="CA4" s="4" t="s">
         <v>12</v>
       </c>
       <c r="CB4" s="23"/>
-      <c r="CC4" s="5"/>
+      <c r="CC4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="CD4" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="CE4" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="CF4" s="15" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="5" spans="1:81" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -2222,25 +2256,44 @@
       <c r="BR5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="BS5" s="21"/>
+      <c r="BS5" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="BT5" s="8" t="s">
         <v>12</v>
       </c>
       <c r="BU5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="BV5" s="22"/>
+      <c r="BV5" s="8" t="s">
+        <v>12</v>
+      </c>
       <c r="BW5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="BX5" s="23"/>
-      <c r="BY5" s="5"/>
-      <c r="BZ5" s="23"/>
-      <c r="CA5" s="5"/>
+      <c r="BX5" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="BY5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="BZ5" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="CA5" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="CB5" s="23"/>
       <c r="CC5" s="5"/>
+      <c r="CD5" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="CE5" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="CF5" s="16"/>
     </row>
-    <row r="6" spans="1:81" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -2469,15 +2522,28 @@
       <c r="BX6" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="BY6" s="5"/>
-      <c r="BZ6" s="23"/>
+      <c r="BY6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="BZ6" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="CA6" s="4" t="s">
         <v>12</v>
       </c>
       <c r="CB6" s="23"/>
       <c r="CC6" s="5"/>
+      <c r="CD6" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="CE6" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="CF6" s="15" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="7" spans="1:81" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>4</v>
       </c>
@@ -2645,8 +2711,11 @@
       <c r="CA7" s="5"/>
       <c r="CB7" s="23"/>
       <c r="CC7" s="5"/>
+      <c r="CD7" s="16"/>
+      <c r="CE7" s="24"/>
+      <c r="CF7" s="16"/>
     </row>
-    <row r="8" spans="1:81" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>5</v>
       </c>
@@ -2872,7 +2941,9 @@
       <c r="BW8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="BX8" s="23"/>
+      <c r="BX8" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="BY8" s="4" t="s">
         <v>12</v>
       </c>
@@ -2884,8 +2955,11 @@
       </c>
       <c r="CB8" s="23"/>
       <c r="CC8" s="5"/>
+      <c r="CD8" s="16"/>
+      <c r="CE8" s="24"/>
+      <c r="CF8" s="16"/>
     </row>
-    <row r="9" spans="1:81" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>6</v>
       </c>
@@ -3037,8 +3111,11 @@
       <c r="CA9" s="5"/>
       <c r="CB9" s="23"/>
       <c r="CC9" s="5"/>
+      <c r="CD9" s="16"/>
+      <c r="CE9" s="24"/>
+      <c r="CF9" s="16"/>
     </row>
-    <row r="10" spans="1:81" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>7</v>
       </c>
@@ -3267,15 +3344,32 @@
       <c r="BX10" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="BY10" s="5"/>
-      <c r="BZ10" s="23"/>
+      <c r="BY10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="BZ10" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="CA10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="CB10" s="23"/>
-      <c r="CC10" s="5"/>
+      <c r="CB10" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="CC10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="CD10" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="CE10" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="CF10" s="15" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="11" spans="1:81" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>8</v>
       </c>
@@ -3407,8 +3501,11 @@
       <c r="CA11" s="5"/>
       <c r="CB11" s="23"/>
       <c r="CC11" s="5"/>
+      <c r="CD11" s="16"/>
+      <c r="CE11" s="24"/>
+      <c r="CF11" s="16"/>
     </row>
-    <row r="12" spans="1:81" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>9</v>
       </c>
@@ -3643,13 +3740,24 @@
       <c r="BZ12" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="CA12" s="5"/>
+      <c r="CA12" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="CB12" s="23"/>
       <c r="CC12" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="CD12" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="CE12" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="CF12" s="15" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="13" spans="1:81" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>10</v>
       </c>
@@ -3805,8 +3913,11 @@
       <c r="CA13" s="5"/>
       <c r="CB13" s="23"/>
       <c r="CC13" s="5"/>
+      <c r="CD13" s="16"/>
+      <c r="CE13" s="24"/>
+      <c r="CF13" s="16"/>
     </row>
-    <row r="14" spans="1:81" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>11</v>
       </c>
@@ -4026,18 +4137,25 @@
       <c r="BU14" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="BV14" s="22"/>
+      <c r="BV14" s="8" t="s">
+        <v>12</v>
+      </c>
       <c r="BW14" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="BX14" s="23"/>
+      <c r="BX14" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="BY14" s="5"/>
       <c r="BZ14" s="23"/>
       <c r="CA14" s="5"/>
       <c r="CB14" s="23"/>
       <c r="CC14" s="5"/>
+      <c r="CD14" s="16"/>
+      <c r="CE14" s="24"/>
+      <c r="CF14" s="16"/>
     </row>
-    <row r="15" spans="1:81" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>12</v>
       </c>
@@ -4273,8 +4391,13 @@
       </c>
       <c r="CB15" s="23"/>
       <c r="CC15" s="5"/>
+      <c r="CD15" s="16"/>
+      <c r="CE15" s="24"/>
+      <c r="CF15" s="15" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="16" spans="1:81" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>13</v>
       </c>
@@ -4482,8 +4605,11 @@
       <c r="CA16" s="5"/>
       <c r="CB16" s="23"/>
       <c r="CC16" s="5"/>
+      <c r="CD16" s="16"/>
+      <c r="CE16" s="24"/>
+      <c r="CF16" s="16"/>
     </row>
-    <row r="17" spans="1:81" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>14</v>
       </c>
@@ -4675,8 +4801,11 @@
       <c r="CA17" s="5"/>
       <c r="CB17" s="23"/>
       <c r="CC17" s="5"/>
+      <c r="CD17" s="16"/>
+      <c r="CE17" s="24"/>
+      <c r="CF17" s="16"/>
     </row>
-    <row r="18" spans="1:81" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>15</v>
       </c>
@@ -4886,8 +5015,11 @@
       <c r="CA18" s="5"/>
       <c r="CB18" s="23"/>
       <c r="CC18" s="5"/>
+      <c r="CD18" s="16"/>
+      <c r="CE18" s="24"/>
+      <c r="CF18" s="16"/>
     </row>
-    <row r="19" spans="1:81" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>16</v>
       </c>
@@ -5108,15 +5240,26 @@
         <v>12</v>
       </c>
       <c r="BX19" s="23"/>
-      <c r="BY19" s="5"/>
-      <c r="BZ19" s="23"/>
+      <c r="BY19" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="BZ19" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="CA19" s="4" t="s">
         <v>12</v>
       </c>
       <c r="CB19" s="23"/>
       <c r="CC19" s="5"/>
+      <c r="CD19" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="CE19" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="CF19" s="16"/>
     </row>
-    <row r="20" spans="1:81" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>17</v>
       </c>
@@ -5340,14 +5483,19 @@
       <c r="BW20" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="BX20" s="23"/>
+      <c r="BX20" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="BY20" s="5"/>
       <c r="BZ20" s="23"/>
       <c r="CA20" s="5"/>
       <c r="CB20" s="23"/>
       <c r="CC20" s="5"/>
+      <c r="CD20" s="16"/>
+      <c r="CE20" s="24"/>
+      <c r="CF20" s="16"/>
     </row>
-    <row r="21" spans="1:81" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>18</v>
       </c>
@@ -5543,8 +5691,11 @@
       <c r="CA21" s="5"/>
       <c r="CB21" s="23"/>
       <c r="CC21" s="5"/>
+      <c r="CD21" s="16"/>
+      <c r="CE21" s="24"/>
+      <c r="CF21" s="16"/>
     </row>
-    <row r="22" spans="1:81" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>19</v>
       </c>
@@ -5754,7 +5905,9 @@
       <c r="BU22" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="BV22" s="22"/>
+      <c r="BV22" s="8" t="s">
+        <v>12</v>
+      </c>
       <c r="BW22" s="7" t="s">
         <v>12</v>
       </c>
@@ -5764,8 +5917,11 @@
       <c r="CA22" s="5"/>
       <c r="CB22" s="23"/>
       <c r="CC22" s="5"/>
+      <c r="CD22" s="16"/>
+      <c r="CE22" s="24"/>
+      <c r="CF22" s="16"/>
     </row>
-    <row r="23" spans="1:81" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>20</v>
       </c>
@@ -5929,8 +6085,11 @@
       <c r="CA23" s="5"/>
       <c r="CB23" s="23"/>
       <c r="CC23" s="5"/>
+      <c r="CD23" s="16"/>
+      <c r="CE23" s="24"/>
+      <c r="CF23" s="16"/>
     </row>
-    <row r="24" spans="1:81" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>21</v>
       </c>
@@ -6084,8 +6243,11 @@
       <c r="CA24" s="5"/>
       <c r="CB24" s="23"/>
       <c r="CC24" s="5"/>
+      <c r="CD24" s="16"/>
+      <c r="CE24" s="24"/>
+      <c r="CF24" s="16"/>
     </row>
-    <row r="25" spans="1:81" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>22</v>
       </c>
@@ -6317,8 +6479,13 @@
       <c r="CA25" s="5"/>
       <c r="CB25" s="23"/>
       <c r="CC25" s="5"/>
+      <c r="CD25" s="16"/>
+      <c r="CE25" s="24"/>
+      <c r="CF25" s="15" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="26" spans="1:81" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>23</v>
       </c>
@@ -6556,12 +6723,23 @@
       <c r="CA26" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="CB26" s="23"/>
+      <c r="CB26" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="CC26" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="CD26" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="CE26" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="CF26" s="15" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="27" spans="1:81" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>24</v>
       </c>
@@ -6803,8 +6981,11 @@
       <c r="CC27" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="CD27" s="16"/>
+      <c r="CE27" s="24"/>
+      <c r="CF27" s="16"/>
     </row>
-    <row r="28" spans="1:81" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>25</v>
       </c>
@@ -7006,7 +7187,9 @@
       <c r="BU28" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="BV28" s="22"/>
+      <c r="BV28" s="8" t="s">
+        <v>12</v>
+      </c>
       <c r="BW28" s="7" t="s">
         <v>12</v>
       </c>
@@ -7015,11 +7198,18 @@
       </c>
       <c r="BY28" s="5"/>
       <c r="BZ28" s="23"/>
-      <c r="CA28" s="5"/>
+      <c r="CA28" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="CB28" s="23"/>
       <c r="CC28" s="5"/>
+      <c r="CD28" s="16"/>
+      <c r="CE28" s="24"/>
+      <c r="CF28" s="15" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="29" spans="1:81" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>26</v>
       </c>
@@ -7249,8 +7439,11 @@
       </c>
       <c r="CB29" s="23"/>
       <c r="CC29" s="5"/>
+      <c r="CD29" s="16"/>
+      <c r="CE29" s="24"/>
+      <c r="CF29" s="16"/>
     </row>
-    <row r="30" spans="1:81" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>27</v>
       </c>
@@ -7374,8 +7567,11 @@
       <c r="CA30" s="5"/>
       <c r="CB30" s="23"/>
       <c r="CC30" s="5"/>
+      <c r="CD30" s="16"/>
+      <c r="CE30" s="24"/>
+      <c r="CF30" s="16"/>
     </row>
-    <row r="31" spans="1:81" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>28</v>
       </c>
@@ -7555,8 +7751,11 @@
       <c r="CA31" s="5"/>
       <c r="CB31" s="23"/>
       <c r="CC31" s="5"/>
+      <c r="CD31" s="16"/>
+      <c r="CE31" s="24"/>
+      <c r="CF31" s="16"/>
     </row>
-    <row r="32" spans="1:81" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>29</v>
       </c>
@@ -7794,10 +7993,23 @@
       <c r="CA32" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="CB32" s="23"/>
-      <c r="CC32" s="5"/>
+      <c r="CB32" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="CC32" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="CD32" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="CE32" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="CF32" s="15" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="33" spans="1:81" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>30</v>
       </c>
@@ -7967,8 +8179,11 @@
       <c r="CA33" s="5"/>
       <c r="CB33" s="23"/>
       <c r="CC33" s="5"/>
+      <c r="CD33" s="16"/>
+      <c r="CE33" s="24"/>
+      <c r="CF33" s="16"/>
     </row>
-    <row r="34" spans="1:81" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>31</v>
       </c>
@@ -8195,13 +8410,22 @@
       <c r="BX34" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="BY34" s="5"/>
-      <c r="BZ34" s="23"/>
-      <c r="CA34" s="5"/>
+      <c r="BY34" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="BZ34" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="CA34" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="CB34" s="23"/>
       <c r="CC34" s="5"/>
+      <c r="CD34" s="16"/>
+      <c r="CE34" s="24"/>
+      <c r="CF34" s="16"/>
     </row>
-    <row r="35" spans="1:81" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>32</v>
       </c>
@@ -8415,14 +8639,33 @@
       <c r="BW35" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="BX35" s="23"/>
-      <c r="BY35" s="5"/>
-      <c r="BZ35" s="23"/>
-      <c r="CA35" s="5"/>
-      <c r="CB35" s="23"/>
-      <c r="CC35" s="5"/>
+      <c r="BX35" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="BY35" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="BZ35" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="CA35" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="CB35" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="CC35" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="CD35" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="CE35" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="CF35" s="16"/>
     </row>
-    <row r="36" spans="1:81" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>33</v>
       </c>
@@ -8660,8 +8903,15 @@
       <c r="CA36" s="5"/>
       <c r="CB36" s="23"/>
       <c r="CC36" s="5"/>
+      <c r="CD36" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="CE36" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="CF36" s="16"/>
     </row>
-    <row r="37" spans="1:81" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>34</v>
       </c>
@@ -8891,8 +9141,11 @@
       <c r="CA37" s="5"/>
       <c r="CB37" s="23"/>
       <c r="CC37" s="5"/>
+      <c r="CD37" s="16"/>
+      <c r="CE37" s="24"/>
+      <c r="CF37" s="16"/>
     </row>
-    <row r="38" spans="1:81" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>35</v>
       </c>
@@ -9084,26 +9337,29 @@
       <c r="CA38" s="5"/>
       <c r="CB38" s="23"/>
       <c r="CC38" s="5"/>
+      <c r="CD38" s="16"/>
+      <c r="CE38" s="24"/>
+      <c r="CF38" s="16"/>
     </row>
-    <row r="40" spans="1:81" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D40" s="38" t="s">
+    <row r="40" spans="1:84" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D40" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="E40" s="38"/>
-      <c r="F40" s="38"/>
-      <c r="G40" s="38"/>
-      <c r="H40" s="38"/>
-      <c r="I40" s="38"/>
-      <c r="J40" s="38"/>
-      <c r="K40" s="38"/>
-      <c r="L40" s="38"/>
-      <c r="M40" s="38"/>
-      <c r="N40" s="38"/>
-      <c r="O40" s="36" t="s">
+      <c r="E40" s="35"/>
+      <c r="F40" s="35"/>
+      <c r="G40" s="35"/>
+      <c r="H40" s="35"/>
+      <c r="I40" s="35"/>
+      <c r="J40" s="35"/>
+      <c r="K40" s="35"/>
+      <c r="L40" s="35"/>
+      <c r="M40" s="35"/>
+      <c r="N40" s="35"/>
+      <c r="O40" s="38" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="41" spans="1:81" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:84" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D41" s="17" t="s">
         <v>7</v>
       </c>
@@ -9137,9 +9393,9 @@
       <c r="N41" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="O41" s="37"/>
+      <c r="O41" s="39"/>
     </row>
-    <row r="42" spans="1:81" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:84" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D42" s="2">
         <v>16</v>
       </c>
@@ -9165,7 +9421,7 @@
         <v>5</v>
       </c>
       <c r="L42" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M42" s="2">
         <v>7</v>
@@ -9175,21 +9431,14 @@
       </c>
       <c r="O42" s="2">
         <f>SUM(D42:N42)</f>
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
-    <row r="43" spans="1:81" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="1:81" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="1:81" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:84" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="1:84" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:84" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:G1"/>
-    <mergeCell ref="H1:O1"/>
-    <mergeCell ref="BO1:BR1"/>
-    <mergeCell ref="BL1:BN1"/>
-    <mergeCell ref="BX1:CC1"/>
+  <mergeCells count="20">
     <mergeCell ref="O40:O41"/>
     <mergeCell ref="D40:N40"/>
     <mergeCell ref="AH1:AL1"/>
@@ -9201,7 +9450,15 @@
     <mergeCell ref="BA1:BF1"/>
     <mergeCell ref="AP1:AT1"/>
     <mergeCell ref="AM1:AO1"/>
+    <mergeCell ref="BX1:CC1"/>
     <mergeCell ref="BS1:BW1"/>
+    <mergeCell ref="CD1:CF1"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="H1:O1"/>
+    <mergeCell ref="BO1:BR1"/>
+    <mergeCell ref="BL1:BN1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B4:B38">

</xml_diff>

<commit_message>
Added HTTP To Listen Log For Quick Access, Fixed Assignment Collection Not Updating Bug, Leaderboard Page Created, Styled Leaderboard Page, Contributor Page Created & Styled Contributor Page
</commit_message>
<xml_diff>
--- a/python/List Tugas Gabunggan.xlsx
+++ b/python/List Tugas Gabunggan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\Web Dev Related Stuff\Web Dev\Web Laporan V.3\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E66180-6EF1-4F04-BB84-638E13526E31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{716B6A2B-D06F-4F77-9504-68A6D66343CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12456" yWindow="1848" windowWidth="10584" windowHeight="8328" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2429" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2444" uniqueCount="159">
   <si>
     <t>No.</t>
   </si>
@@ -778,31 +778,31 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1117,7 +1117,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="BX4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="BX10" sqref="BX10:CF10"/>
+      <selection pane="bottomRight" activeCell="CB36" sqref="CB36:CC36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1172,10 +1172,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:84" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="33" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="36" t="s">
@@ -1185,30 +1185,30 @@
       <c r="E1" s="36"/>
       <c r="F1" s="36"/>
       <c r="G1" s="36"/>
-      <c r="H1" s="37" t="s">
+      <c r="H1" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="32" t="s">
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
+      <c r="P1" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="31" t="s">
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
+      <c r="T1" s="35"/>
+      <c r="U1" s="35"/>
+      <c r="V1" s="35"/>
+      <c r="W1" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="31"/>
+      <c r="X1" s="37"/>
+      <c r="Y1" s="37"/>
       <c r="Z1" s="36" t="s">
         <v>85</v>
       </c>
@@ -1219,25 +1219,25 @@
       <c r="AE1" s="36"/>
       <c r="AF1" s="36"/>
       <c r="AG1" s="36"/>
-      <c r="AH1" s="37" t="s">
+      <c r="AH1" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="AI1" s="37"/>
-      <c r="AJ1" s="37"/>
-      <c r="AK1" s="37"/>
-      <c r="AL1" s="37"/>
-      <c r="AM1" s="32" t="s">
+      <c r="AI1" s="34"/>
+      <c r="AJ1" s="34"/>
+      <c r="AK1" s="34"/>
+      <c r="AL1" s="34"/>
+      <c r="AM1" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="AN1" s="32"/>
-      <c r="AO1" s="32"/>
-      <c r="AP1" s="31" t="s">
+      <c r="AN1" s="35"/>
+      <c r="AO1" s="35"/>
+      <c r="AP1" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="AQ1" s="31"/>
-      <c r="AR1" s="31"/>
-      <c r="AS1" s="31"/>
-      <c r="AT1" s="31"/>
+      <c r="AQ1" s="37"/>
+      <c r="AR1" s="37"/>
+      <c r="AS1" s="37"/>
+      <c r="AT1" s="37"/>
       <c r="AU1" s="36" t="s">
         <v>114</v>
       </c>
@@ -1246,20 +1246,20 @@
       <c r="AX1" s="36"/>
       <c r="AY1" s="36"/>
       <c r="AZ1" s="36"/>
-      <c r="BA1" s="37" t="s">
+      <c r="BA1" s="34" t="s">
         <v>120</v>
       </c>
-      <c r="BB1" s="37"/>
-      <c r="BC1" s="37"/>
-      <c r="BD1" s="37"/>
-      <c r="BE1" s="37"/>
-      <c r="BF1" s="37"/>
-      <c r="BG1" s="32" t="s">
+      <c r="BB1" s="34"/>
+      <c r="BC1" s="34"/>
+      <c r="BD1" s="34"/>
+      <c r="BE1" s="34"/>
+      <c r="BF1" s="34"/>
+      <c r="BG1" s="35" t="s">
         <v>126</v>
       </c>
-      <c r="BH1" s="32"/>
-      <c r="BI1" s="32"/>
-      <c r="BJ1" s="32"/>
+      <c r="BH1" s="35"/>
+      <c r="BI1" s="35"/>
+      <c r="BJ1" s="35"/>
       <c r="BK1" s="29" t="s">
         <v>132</v>
       </c>
@@ -1268,36 +1268,36 @@
       </c>
       <c r="BM1" s="36"/>
       <c r="BN1" s="36"/>
-      <c r="BO1" s="37" t="s">
+      <c r="BO1" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="BP1" s="37"/>
-      <c r="BQ1" s="37"/>
-      <c r="BR1" s="37"/>
-      <c r="BS1" s="32" t="s">
+      <c r="BP1" s="34"/>
+      <c r="BQ1" s="34"/>
+      <c r="BR1" s="34"/>
+      <c r="BS1" s="35" t="s">
         <v>146</v>
       </c>
-      <c r="BT1" s="32"/>
-      <c r="BU1" s="32"/>
-      <c r="BV1" s="32"/>
-      <c r="BW1" s="32"/>
-      <c r="BX1" s="31" t="s">
+      <c r="BT1" s="35"/>
+      <c r="BU1" s="35"/>
+      <c r="BV1" s="35"/>
+      <c r="BW1" s="35"/>
+      <c r="BX1" s="37" t="s">
         <v>148</v>
       </c>
-      <c r="BY1" s="31"/>
-      <c r="BZ1" s="31"/>
-      <c r="CA1" s="31"/>
-      <c r="CB1" s="31"/>
-      <c r="CC1" s="31"/>
-      <c r="CD1" s="33" t="s">
+      <c r="BY1" s="37"/>
+      <c r="BZ1" s="37"/>
+      <c r="CA1" s="37"/>
+      <c r="CB1" s="37"/>
+      <c r="CC1" s="37"/>
+      <c r="CD1" s="38" t="s">
         <v>155</v>
       </c>
-      <c r="CE1" s="34"/>
-      <c r="CF1" s="34"/>
+      <c r="CE1" s="39"/>
+      <c r="CF1" s="39"/>
     </row>
     <row r="2" spans="1:84" ht="18" x14ac:dyDescent="0.3">
-      <c r="A2" s="35"/>
-      <c r="B2" s="35"/>
+      <c r="A2" s="33"/>
+      <c r="B2" s="33"/>
       <c r="C2" s="26" t="s">
         <v>2</v>
       </c>
@@ -1546,8 +1546,8 @@
       </c>
     </row>
     <row r="3" spans="1:84" ht="18" x14ac:dyDescent="0.3">
-      <c r="A3" s="35"/>
-      <c r="B3" s="35"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="33"/>
       <c r="C3" s="13" t="s">
         <v>58</v>
       </c>
@@ -2031,7 +2031,9 @@
       <c r="CA4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="CB4" s="23"/>
+      <c r="CB4" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="CC4" s="4" t="s">
         <v>12</v>
       </c>
@@ -2955,9 +2957,15 @@
       </c>
       <c r="CB8" s="23"/>
       <c r="CC8" s="5"/>
-      <c r="CD8" s="16"/>
-      <c r="CE8" s="24"/>
-      <c r="CF8" s="16"/>
+      <c r="CD8" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="CE8" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="CF8" s="15" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="9" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
@@ -5486,13 +5494,25 @@
       <c r="BX20" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="BY20" s="5"/>
-      <c r="BZ20" s="23"/>
+      <c r="BY20" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="BZ20" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="CA20" s="5"/>
-      <c r="CB20" s="23"/>
-      <c r="CC20" s="5"/>
-      <c r="CD20" s="16"/>
-      <c r="CE20" s="24"/>
+      <c r="CB20" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="CC20" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="CD20" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="CE20" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="CF20" s="16"/>
     </row>
     <row r="21" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
@@ -6981,9 +7001,15 @@
       <c r="CC27" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="CD27" s="16"/>
-      <c r="CE27" s="24"/>
-      <c r="CF27" s="16"/>
+      <c r="CD27" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="CE27" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="CF27" s="15" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="28" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
@@ -8900,7 +8926,9 @@
       <c r="BZ36" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="CA36" s="5"/>
+      <c r="CA36" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="CB36" s="23"/>
       <c r="CC36" s="5"/>
       <c r="CD36" s="15" t="s">
@@ -8909,7 +8937,9 @@
       <c r="CE36" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="CF36" s="16"/>
+      <c r="CF36" s="15" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="37" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
@@ -9342,20 +9372,20 @@
       <c r="CF38" s="16"/>
     </row>
     <row r="40" spans="1:84" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D40" s="35" t="s">
+      <c r="D40" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="E40" s="35"/>
-      <c r="F40" s="35"/>
-      <c r="G40" s="35"/>
-      <c r="H40" s="35"/>
-      <c r="I40" s="35"/>
-      <c r="J40" s="35"/>
-      <c r="K40" s="35"/>
-      <c r="L40" s="35"/>
-      <c r="M40" s="35"/>
-      <c r="N40" s="35"/>
-      <c r="O40" s="38" t="s">
+      <c r="E40" s="33"/>
+      <c r="F40" s="33"/>
+      <c r="G40" s="33"/>
+      <c r="H40" s="33"/>
+      <c r="I40" s="33"/>
+      <c r="J40" s="33"/>
+      <c r="K40" s="33"/>
+      <c r="L40" s="33"/>
+      <c r="M40" s="33"/>
+      <c r="N40" s="33"/>
+      <c r="O40" s="31" t="s">
         <v>78</v>
       </c>
     </row>
@@ -9393,7 +9423,7 @@
       <c r="N41" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="O41" s="39"/>
+      <c r="O41" s="32"/>
     </row>
     <row r="42" spans="1:84" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D42" s="2">
@@ -9439,6 +9469,15 @@
     <row r="45" spans="1:84" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="BX1:CC1"/>
+    <mergeCell ref="BS1:BW1"/>
+    <mergeCell ref="CD1:CF1"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="H1:O1"/>
+    <mergeCell ref="BO1:BR1"/>
+    <mergeCell ref="BL1:BN1"/>
     <mergeCell ref="O40:O41"/>
     <mergeCell ref="D40:N40"/>
     <mergeCell ref="AH1:AL1"/>
@@ -9450,15 +9489,6 @@
     <mergeCell ref="BA1:BF1"/>
     <mergeCell ref="AP1:AT1"/>
     <mergeCell ref="AM1:AO1"/>
-    <mergeCell ref="BX1:CC1"/>
-    <mergeCell ref="BS1:BW1"/>
-    <mergeCell ref="CD1:CF1"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:G1"/>
-    <mergeCell ref="H1:O1"/>
-    <mergeCell ref="BO1:BR1"/>
-    <mergeCell ref="BL1:BN1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B4:B38">

</xml_diff>

<commit_message>
Fixed List Of Assignment Data Not Accurate Bug
</commit_message>
<xml_diff>
--- a/python/List Tugas Gabunggan.xlsx
+++ b/python/List Tugas Gabunggan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\Web Dev Related Stuff\Web Dev\Web Laporan V.3\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{716B6A2B-D06F-4F77-9504-68A6D66343CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76E86FDC-322F-4285-9087-8EF5F3FA6E9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12456" yWindow="1848" windowWidth="10584" windowHeight="8328" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2444" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2455" uniqueCount="161">
   <si>
     <t>No.</t>
   </si>
@@ -505,6 +505,12 @@
   </si>
   <si>
     <t>BING9</t>
+  </si>
+  <si>
+    <t>Minggu Ke-18</t>
+  </si>
+  <si>
+    <t>PPL5</t>
   </si>
 </sst>
 </file>
@@ -688,7 +694,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -778,31 +784,34 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1111,13 +1120,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CF45"/>
+  <dimension ref="A1:CG45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="BX4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="CB36" sqref="CB36:CC36"/>
+      <selection pane="bottomRight" activeCell="CG6" sqref="A1:CG38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1168,136 +1177,140 @@
     <col min="79" max="81" width="9.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="82" max="83" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="84" max="84" width="9.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="85" max="16384" width="8.88671875" style="1"/>
+    <col min="85" max="85" width="16.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="86" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:84" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:85" ht="18" x14ac:dyDescent="0.3">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="34" t="s">
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="35" t="s">
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="35"/>
-      <c r="S1" s="35"/>
-      <c r="T1" s="35"/>
-      <c r="U1" s="35"/>
-      <c r="V1" s="35"/>
-      <c r="W1" s="37" t="s">
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="33"/>
+      <c r="U1" s="33"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="X1" s="37"/>
-      <c r="Y1" s="37"/>
-      <c r="Z1" s="36" t="s">
+      <c r="X1" s="32"/>
+      <c r="Y1" s="32"/>
+      <c r="Z1" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="AA1" s="36"/>
-      <c r="AB1" s="36"/>
-      <c r="AC1" s="36"/>
-      <c r="AD1" s="36"/>
-      <c r="AE1" s="36"/>
-      <c r="AF1" s="36"/>
-      <c r="AG1" s="36"/>
-      <c r="AH1" s="34" t="s">
+      <c r="AA1" s="37"/>
+      <c r="AB1" s="37"/>
+      <c r="AC1" s="37"/>
+      <c r="AD1" s="37"/>
+      <c r="AE1" s="37"/>
+      <c r="AF1" s="37"/>
+      <c r="AG1" s="37"/>
+      <c r="AH1" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="AI1" s="34"/>
-      <c r="AJ1" s="34"/>
-      <c r="AK1" s="34"/>
-      <c r="AL1" s="34"/>
-      <c r="AM1" s="35" t="s">
+      <c r="AI1" s="38"/>
+      <c r="AJ1" s="38"/>
+      <c r="AK1" s="38"/>
+      <c r="AL1" s="38"/>
+      <c r="AM1" s="33" t="s">
         <v>100</v>
       </c>
-      <c r="AN1" s="35"/>
-      <c r="AO1" s="35"/>
-      <c r="AP1" s="37" t="s">
+      <c r="AN1" s="33"/>
+      <c r="AO1" s="33"/>
+      <c r="AP1" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="AQ1" s="37"/>
-      <c r="AR1" s="37"/>
-      <c r="AS1" s="37"/>
-      <c r="AT1" s="37"/>
-      <c r="AU1" s="36" t="s">
+      <c r="AQ1" s="32"/>
+      <c r="AR1" s="32"/>
+      <c r="AS1" s="32"/>
+      <c r="AT1" s="32"/>
+      <c r="AU1" s="37" t="s">
         <v>114</v>
       </c>
-      <c r="AV1" s="36"/>
-      <c r="AW1" s="36"/>
-      <c r="AX1" s="36"/>
-      <c r="AY1" s="36"/>
-      <c r="AZ1" s="36"/>
-      <c r="BA1" s="34" t="s">
+      <c r="AV1" s="37"/>
+      <c r="AW1" s="37"/>
+      <c r="AX1" s="37"/>
+      <c r="AY1" s="37"/>
+      <c r="AZ1" s="37"/>
+      <c r="BA1" s="38" t="s">
         <v>120</v>
       </c>
-      <c r="BB1" s="34"/>
-      <c r="BC1" s="34"/>
-      <c r="BD1" s="34"/>
-      <c r="BE1" s="34"/>
-      <c r="BF1" s="34"/>
-      <c r="BG1" s="35" t="s">
+      <c r="BB1" s="38"/>
+      <c r="BC1" s="38"/>
+      <c r="BD1" s="38"/>
+      <c r="BE1" s="38"/>
+      <c r="BF1" s="38"/>
+      <c r="BG1" s="33" t="s">
         <v>126</v>
       </c>
-      <c r="BH1" s="35"/>
-      <c r="BI1" s="35"/>
-      <c r="BJ1" s="35"/>
+      <c r="BH1" s="33"/>
+      <c r="BI1" s="33"/>
+      <c r="BJ1" s="33"/>
       <c r="BK1" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="BL1" s="36" t="s">
+      <c r="BL1" s="37" t="s">
         <v>134</v>
       </c>
-      <c r="BM1" s="36"/>
-      <c r="BN1" s="36"/>
-      <c r="BO1" s="34" t="s">
+      <c r="BM1" s="37"/>
+      <c r="BN1" s="37"/>
+      <c r="BO1" s="38" t="s">
         <v>138</v>
       </c>
-      <c r="BP1" s="34"/>
-      <c r="BQ1" s="34"/>
-      <c r="BR1" s="34"/>
-      <c r="BS1" s="35" t="s">
+      <c r="BP1" s="38"/>
+      <c r="BQ1" s="38"/>
+      <c r="BR1" s="38"/>
+      <c r="BS1" s="33" t="s">
         <v>146</v>
       </c>
-      <c r="BT1" s="35"/>
-      <c r="BU1" s="35"/>
-      <c r="BV1" s="35"/>
-      <c r="BW1" s="35"/>
-      <c r="BX1" s="37" t="s">
+      <c r="BT1" s="33"/>
+      <c r="BU1" s="33"/>
+      <c r="BV1" s="33"/>
+      <c r="BW1" s="33"/>
+      <c r="BX1" s="32" t="s">
         <v>148</v>
       </c>
-      <c r="BY1" s="37"/>
-      <c r="BZ1" s="37"/>
-      <c r="CA1" s="37"/>
-      <c r="CB1" s="37"/>
-      <c r="CC1" s="37"/>
-      <c r="CD1" s="38" t="s">
+      <c r="BY1" s="32"/>
+      <c r="BZ1" s="32"/>
+      <c r="CA1" s="32"/>
+      <c r="CB1" s="32"/>
+      <c r="CC1" s="32"/>
+      <c r="CD1" s="34" t="s">
         <v>155</v>
       </c>
-      <c r="CE1" s="39"/>
-      <c r="CF1" s="39"/>
+      <c r="CE1" s="35"/>
+      <c r="CF1" s="35"/>
+      <c r="CG1" s="31" t="s">
+        <v>159</v>
+      </c>
     </row>
-    <row r="2" spans="1:84" ht="18" x14ac:dyDescent="0.3">
-      <c r="A2" s="33"/>
-      <c r="B2" s="33"/>
+    <row r="2" spans="1:85" ht="18" x14ac:dyDescent="0.3">
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
       <c r="C2" s="26" t="s">
         <v>2</v>
       </c>
@@ -1544,10 +1557,13 @@
       <c r="CF2" s="30" t="s">
         <v>4</v>
       </c>
+      <c r="CG2" s="31" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="3" spans="1:84" ht="18" x14ac:dyDescent="0.3">
-      <c r="A3" s="33"/>
-      <c r="B3" s="33"/>
+    <row r="3" spans="1:85" ht="18" x14ac:dyDescent="0.3">
+      <c r="A3" s="36"/>
+      <c r="B3" s="36"/>
       <c r="C3" s="13" t="s">
         <v>58</v>
       </c>
@@ -1794,8 +1810,11 @@
       <c r="CF3" s="13" t="s">
         <v>158</v>
       </c>
+      <c r="CG3" s="9" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="4" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:85" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -2046,8 +2065,9 @@
       <c r="CF4" s="15" t="s">
         <v>12</v>
       </c>
+      <c r="CG4" s="25"/>
     </row>
-    <row r="5" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:85" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -2294,8 +2314,9 @@
         <v>12</v>
       </c>
       <c r="CF5" s="16"/>
+      <c r="CG5" s="25"/>
     </row>
-    <row r="6" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:85" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -2533,7 +2554,9 @@
       <c r="CA6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="CB6" s="23"/>
+      <c r="CB6" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="CC6" s="5"/>
       <c r="CD6" s="15" t="s">
         <v>12</v>
@@ -2544,8 +2567,9 @@
       <c r="CF6" s="15" t="s">
         <v>12</v>
       </c>
+      <c r="CG6" s="25"/>
     </row>
-    <row r="7" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:85" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>4</v>
       </c>
@@ -2716,8 +2740,9 @@
       <c r="CD7" s="16"/>
       <c r="CE7" s="24"/>
       <c r="CF7" s="16"/>
+      <c r="CG7" s="25"/>
     </row>
-    <row r="8" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:85" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>5</v>
       </c>
@@ -2966,8 +2991,9 @@
       <c r="CF8" s="15" t="s">
         <v>12</v>
       </c>
+      <c r="CG8" s="25"/>
     </row>
-    <row r="9" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:85" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>6</v>
       </c>
@@ -3122,8 +3148,9 @@
       <c r="CD9" s="16"/>
       <c r="CE9" s="24"/>
       <c r="CF9" s="16"/>
+      <c r="CG9" s="25"/>
     </row>
-    <row r="10" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:85" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>7</v>
       </c>
@@ -3376,8 +3403,9 @@
       <c r="CF10" s="15" t="s">
         <v>12</v>
       </c>
+      <c r="CG10" s="25"/>
     </row>
-    <row r="11" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:85" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>8</v>
       </c>
@@ -3512,8 +3540,9 @@
       <c r="CD11" s="16"/>
       <c r="CE11" s="24"/>
       <c r="CF11" s="16"/>
+      <c r="CG11" s="25"/>
     </row>
-    <row r="12" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:85" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>9</v>
       </c>
@@ -3764,8 +3793,9 @@
       <c r="CF12" s="15" t="s">
         <v>12</v>
       </c>
+      <c r="CG12" s="25"/>
     </row>
-    <row r="13" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:85" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>10</v>
       </c>
@@ -3924,8 +3954,9 @@
       <c r="CD13" s="16"/>
       <c r="CE13" s="24"/>
       <c r="CF13" s="16"/>
+      <c r="CG13" s="25"/>
     </row>
-    <row r="14" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:85" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>11</v>
       </c>
@@ -4162,8 +4193,9 @@
       <c r="CD14" s="16"/>
       <c r="CE14" s="24"/>
       <c r="CF14" s="16"/>
+      <c r="CG14" s="25"/>
     </row>
-    <row r="15" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:85" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>12</v>
       </c>
@@ -4397,15 +4429,18 @@
       <c r="CA15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="CB15" s="23"/>
+      <c r="CB15" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="CC15" s="5"/>
       <c r="CD15" s="16"/>
       <c r="CE15" s="24"/>
       <c r="CF15" s="15" t="s">
         <v>12</v>
       </c>
+      <c r="CG15" s="25"/>
     </row>
-    <row r="16" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:85" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>13</v>
       </c>
@@ -4616,8 +4651,9 @@
       <c r="CD16" s="16"/>
       <c r="CE16" s="24"/>
       <c r="CF16" s="16"/>
+      <c r="CG16" s="25"/>
     </row>
-    <row r="17" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:85" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>14</v>
       </c>
@@ -4812,8 +4848,9 @@
       <c r="CD17" s="16"/>
       <c r="CE17" s="24"/>
       <c r="CF17" s="16"/>
+      <c r="CG17" s="25"/>
     </row>
-    <row r="18" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:85" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>15</v>
       </c>
@@ -5026,8 +5063,9 @@
       <c r="CD18" s="16"/>
       <c r="CE18" s="24"/>
       <c r="CF18" s="16"/>
+      <c r="CG18" s="25"/>
     </row>
-    <row r="19" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:85" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>16</v>
       </c>
@@ -5266,8 +5304,9 @@
         <v>12</v>
       </c>
       <c r="CF19" s="16"/>
+      <c r="CG19" s="25"/>
     </row>
-    <row r="20" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:85" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>17</v>
       </c>
@@ -5514,8 +5553,9 @@
         <v>12</v>
       </c>
       <c r="CF20" s="16"/>
+      <c r="CG20" s="25"/>
     </row>
-    <row r="21" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:85" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>18</v>
       </c>
@@ -5714,8 +5754,9 @@
       <c r="CD21" s="16"/>
       <c r="CE21" s="24"/>
       <c r="CF21" s="16"/>
+      <c r="CG21" s="25"/>
     </row>
-    <row r="22" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:85" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>19</v>
       </c>
@@ -5940,8 +5981,9 @@
       <c r="CD22" s="16"/>
       <c r="CE22" s="24"/>
       <c r="CF22" s="16"/>
+      <c r="CG22" s="25"/>
     </row>
-    <row r="23" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:85" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>20</v>
       </c>
@@ -6108,8 +6150,9 @@
       <c r="CD23" s="16"/>
       <c r="CE23" s="24"/>
       <c r="CF23" s="16"/>
+      <c r="CG23" s="25"/>
     </row>
-    <row r="24" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:85" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>21</v>
       </c>
@@ -6266,8 +6309,9 @@
       <c r="CD24" s="16"/>
       <c r="CE24" s="24"/>
       <c r="CF24" s="16"/>
+      <c r="CG24" s="25"/>
     </row>
-    <row r="25" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:85" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>22</v>
       </c>
@@ -6504,8 +6548,9 @@
       <c r="CF25" s="15" t="s">
         <v>12</v>
       </c>
+      <c r="CG25" s="25"/>
     </row>
-    <row r="26" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:85" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>23</v>
       </c>
@@ -6758,8 +6803,9 @@
       <c r="CF26" s="15" t="s">
         <v>12</v>
       </c>
+      <c r="CG26" s="25"/>
     </row>
-    <row r="27" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:85" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>24</v>
       </c>
@@ -7010,8 +7056,9 @@
       <c r="CF27" s="15" t="s">
         <v>12</v>
       </c>
+      <c r="CG27" s="25"/>
     </row>
-    <row r="28" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:85" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>25</v>
       </c>
@@ -7234,8 +7281,9 @@
       <c r="CF28" s="15" t="s">
         <v>12</v>
       </c>
+      <c r="CG28" s="25"/>
     </row>
-    <row r="29" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:85" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>26</v>
       </c>
@@ -7468,8 +7516,9 @@
       <c r="CD29" s="16"/>
       <c r="CE29" s="24"/>
       <c r="CF29" s="16"/>
+      <c r="CG29" s="25"/>
     </row>
-    <row r="30" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:85" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>27</v>
       </c>
@@ -7596,8 +7645,9 @@
       <c r="CD30" s="16"/>
       <c r="CE30" s="24"/>
       <c r="CF30" s="16"/>
+      <c r="CG30" s="25"/>
     </row>
-    <row r="31" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:85" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>28</v>
       </c>
@@ -7780,8 +7830,9 @@
       <c r="CD31" s="16"/>
       <c r="CE31" s="24"/>
       <c r="CF31" s="16"/>
+      <c r="CG31" s="25"/>
     </row>
-    <row r="32" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:85" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>29</v>
       </c>
@@ -8034,8 +8085,11 @@
       <c r="CF32" s="15" t="s">
         <v>12</v>
       </c>
+      <c r="CG32" s="10" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="33" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:85" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>30</v>
       </c>
@@ -8208,8 +8262,9 @@
       <c r="CD33" s="16"/>
       <c r="CE33" s="24"/>
       <c r="CF33" s="16"/>
+      <c r="CG33" s="25"/>
     </row>
-    <row r="34" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:85" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>31</v>
       </c>
@@ -8445,13 +8500,24 @@
       <c r="CA34" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="CB34" s="23"/>
-      <c r="CC34" s="5"/>
-      <c r="CD34" s="16"/>
-      <c r="CE34" s="24"/>
-      <c r="CF34" s="16"/>
+      <c r="CB34" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="CC34" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="CD34" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="CE34" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="CF34" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="CG34" s="25"/>
     </row>
-    <row r="35" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:85" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>32</v>
       </c>
@@ -8690,8 +8756,9 @@
         <v>12</v>
       </c>
       <c r="CF35" s="16"/>
+      <c r="CG35" s="25"/>
     </row>
-    <row r="36" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:85" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>33</v>
       </c>
@@ -8940,8 +9007,9 @@
       <c r="CF36" s="15" t="s">
         <v>12</v>
       </c>
+      <c r="CG36" s="25"/>
     </row>
-    <row r="37" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:85" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>34</v>
       </c>
@@ -9174,8 +9242,9 @@
       <c r="CD37" s="16"/>
       <c r="CE37" s="24"/>
       <c r="CF37" s="16"/>
+      <c r="CG37" s="25"/>
     </row>
-    <row r="38" spans="1:84" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:85" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>35</v>
       </c>
@@ -9370,26 +9439,27 @@
       <c r="CD38" s="16"/>
       <c r="CE38" s="24"/>
       <c r="CF38" s="16"/>
+      <c r="CG38" s="25"/>
     </row>
-    <row r="40" spans="1:84" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D40" s="33" t="s">
+    <row r="40" spans="1:85" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D40" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="E40" s="33"/>
-      <c r="F40" s="33"/>
-      <c r="G40" s="33"/>
-      <c r="H40" s="33"/>
-      <c r="I40" s="33"/>
-      <c r="J40" s="33"/>
-      <c r="K40" s="33"/>
-      <c r="L40" s="33"/>
-      <c r="M40" s="33"/>
-      <c r="N40" s="33"/>
-      <c r="O40" s="31" t="s">
+      <c r="E40" s="36"/>
+      <c r="F40" s="36"/>
+      <c r="G40" s="36"/>
+      <c r="H40" s="36"/>
+      <c r="I40" s="36"/>
+      <c r="J40" s="36"/>
+      <c r="K40" s="36"/>
+      <c r="L40" s="36"/>
+      <c r="M40" s="36"/>
+      <c r="N40" s="36"/>
+      <c r="O40" s="39" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="41" spans="1:84" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:85" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D41" s="17" t="s">
         <v>7</v>
       </c>
@@ -9423,14 +9493,14 @@
       <c r="N41" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="O41" s="32"/>
+      <c r="O41" s="40"/>
     </row>
-    <row r="42" spans="1:84" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:85" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D42" s="2">
         <v>16</v>
       </c>
       <c r="E42" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F42" s="2">
         <v>3</v>
@@ -9461,23 +9531,14 @@
       </c>
       <c r="O42" s="2">
         <f>SUM(D42:N42)</f>
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
-    <row r="43" spans="1:84" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="1:84" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="1:84" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:85" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="1:85" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:85" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="BX1:CC1"/>
-    <mergeCell ref="BS1:BW1"/>
-    <mergeCell ref="CD1:CF1"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:G1"/>
-    <mergeCell ref="H1:O1"/>
-    <mergeCell ref="BO1:BR1"/>
-    <mergeCell ref="BL1:BN1"/>
     <mergeCell ref="O40:O41"/>
     <mergeCell ref="D40:N40"/>
     <mergeCell ref="AH1:AL1"/>
@@ -9489,6 +9550,15 @@
     <mergeCell ref="BA1:BF1"/>
     <mergeCell ref="AP1:AT1"/>
     <mergeCell ref="AM1:AO1"/>
+    <mergeCell ref="BX1:CC1"/>
+    <mergeCell ref="BS1:BW1"/>
+    <mergeCell ref="CD1:CF1"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="H1:O1"/>
+    <mergeCell ref="BO1:BR1"/>
+    <mergeCell ref="BL1:BN1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B4:B38">

</xml_diff>

<commit_message>
Fixed Bug When Creating A PAI Assignment & Sort Collections
</commit_message>
<xml_diff>
--- a/python/List Tugas Gabunggan.xlsx
+++ b/python/List Tugas Gabunggan.xlsx
@@ -5,18 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\Web Dev Related Stuff\Web Dev\Web Laporan V.4\python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Program Files\Programs\Web Dev Related Stuff\Web Dev\Web Laporan V.3\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7A8F55-CA1D-4906-BFB0-3CC8BA5DB504}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854B1EEC-2EB4-4310-82F2-5ED5F70F623F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="864" yWindow="2664" windowWidth="17292" windowHeight="8904" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$R$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$38</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="70">
   <si>
     <t>No.</t>
   </si>
@@ -151,13 +151,100 @@
   </si>
   <si>
     <t>ü</t>
+  </si>
+  <si>
+    <t>Tugas 2</t>
+  </si>
+  <si>
+    <t>Tugas 3</t>
+  </si>
+  <si>
+    <t>Tugas 4</t>
+  </si>
+  <si>
+    <t>Tugas 5</t>
+  </si>
+  <si>
+    <t>Tugas 6</t>
+  </si>
+  <si>
+    <t>Tugas 7</t>
+  </si>
+  <si>
+    <t>BASDA1</t>
+  </si>
+  <si>
+    <t>PPL1</t>
+  </si>
+  <si>
+    <t>PBO1</t>
+  </si>
+  <si>
+    <t>BINDO1</t>
+  </si>
+  <si>
+    <t>PAI1</t>
+  </si>
+  <si>
+    <t>BING1</t>
+  </si>
+  <si>
+    <t>Tugas 8</t>
+  </si>
+  <si>
+    <t>PKN1</t>
+  </si>
+  <si>
+    <t>Minggu Ke-2</t>
+  </si>
+  <si>
+    <t>MAT2</t>
+  </si>
+  <si>
+    <t>Tugas 9</t>
+  </si>
+  <si>
+    <t>PKK1</t>
+  </si>
+  <si>
+    <t>NON-MUS</t>
+  </si>
+  <si>
+    <t>MAT3</t>
+  </si>
+  <si>
+    <t>BASDA2</t>
+  </si>
+  <si>
+    <t>PKN2</t>
+  </si>
+  <si>
+    <t>PKK2</t>
+  </si>
+  <si>
+    <t>Minggu Ke-3</t>
+  </si>
+  <si>
+    <t>PJOK1</t>
+  </si>
+  <si>
+    <t>Minggu Ke-4</t>
+  </si>
+  <si>
+    <t>BINDO2</t>
+  </si>
+  <si>
+    <t>BASDA3</t>
+  </si>
+  <si>
+    <t>MAT4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -199,8 +286,39 @@
       <name val="Wingdings"/>
       <charset val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Wingdings"/>
+      <charset val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -213,8 +331,44 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA9FA7D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6DC240"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE35DB4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF296D2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF1DAADE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5ED4FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -237,11 +391,57 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -259,7 +459,76 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -568,28 +837,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:T45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A26" sqref="A26:C26"/>
+      <selection pane="bottomRight" activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="10" width="9.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="9.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="18" width="9.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="24" width="9.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="9.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="18" width="9.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="24" width="9.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="10.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="26" max="27" width="9.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="28" max="29" width="9.77734375" style="2" bestFit="1" customWidth="1"/>
@@ -616,50 +889,217 @@
     <col min="64" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:20" ht="18" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="23" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.3">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
+      <c r="D1" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="S1" s="29"/>
+      <c r="T1" s="30"/>
+    </row>
+    <row r="2" spans="1:20" ht="18" x14ac:dyDescent="0.3">
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.3">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
+      <c r="D2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="M2" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="O2" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="P2" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q2" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="R2" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="S2" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="T2" s="21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="18" x14ac:dyDescent="0.3">
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D3" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="M3" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="N3" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="O3" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="P3" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q3" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="R3" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="S3" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="T3" s="22" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="5"/>
-    </row>
-    <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C4" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L4" s="10"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="19"/>
+      <c r="S4" s="20"/>
+      <c r="T4" s="19"/>
+    </row>
+    <row r="5" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="5"/>
-    </row>
-    <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C5" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L5" s="10"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="19"/>
+      <c r="S5" s="20"/>
+      <c r="T5" s="19"/>
+    </row>
+    <row r="6" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>3</v>
       </c>
@@ -667,8 +1107,27 @@
         <v>5</v>
       </c>
       <c r="C6" s="5"/>
-    </row>
-    <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D6" s="10"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L6" s="10"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="19"/>
+      <c r="S6" s="20"/>
+      <c r="T6" s="19"/>
+    </row>
+    <row r="7" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>4</v>
       </c>
@@ -676,17 +1135,57 @@
         <v>6</v>
       </c>
       <c r="C7" s="5"/>
-    </row>
-    <row r="8" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D7" s="10"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L7" s="10"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="20"/>
+      <c r="T7" s="19"/>
+    </row>
+    <row r="8" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>5</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="5"/>
-    </row>
-    <row r="9" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C8" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L8" s="10"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="16"/>
+      <c r="R8" s="19"/>
+      <c r="S8" s="20"/>
+      <c r="T8" s="19"/>
+    </row>
+    <row r="9" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>6</v>
       </c>
@@ -694,17 +1193,57 @@
         <v>8</v>
       </c>
       <c r="C9" s="5"/>
-    </row>
-    <row r="10" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D9" s="10"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L9" s="10"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="19"/>
+      <c r="S9" s="20"/>
+      <c r="T9" s="19"/>
+    </row>
+    <row r="10" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>7</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="5"/>
-    </row>
-    <row r="11" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L10" s="10"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="16"/>
+      <c r="R10" s="19"/>
+      <c r="S10" s="20"/>
+      <c r="T10" s="19"/>
+    </row>
+    <row r="11" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>8</v>
       </c>
@@ -712,17 +1251,57 @@
         <v>10</v>
       </c>
       <c r="C11" s="5"/>
-    </row>
-    <row r="12" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D11" s="10"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L11" s="10"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="16"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="20"/>
+      <c r="T11" s="19"/>
+    </row>
+    <row r="12" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>9</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="5"/>
-    </row>
-    <row r="13" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C12" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="10"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L12" s="10"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="16"/>
+      <c r="R12" s="19"/>
+      <c r="S12" s="20"/>
+      <c r="T12" s="19"/>
+    </row>
+    <row r="13" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>10</v>
       </c>
@@ -730,8 +1309,27 @@
         <v>12</v>
       </c>
       <c r="C13" s="5"/>
-    </row>
-    <row r="14" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D13" s="10"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L13" s="10"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="16"/>
+      <c r="R13" s="19"/>
+      <c r="S13" s="20"/>
+      <c r="T13" s="19"/>
+    </row>
+    <row r="14" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>11</v>
       </c>
@@ -739,17 +1337,59 @@
         <v>13</v>
       </c>
       <c r="C14" s="5"/>
-    </row>
-    <row r="15" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D14" s="10"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L14" s="10"/>
+      <c r="M14" s="16"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="16"/>
+      <c r="R14" s="19"/>
+      <c r="S14" s="20"/>
+      <c r="T14" s="19"/>
+    </row>
+    <row r="15" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>12</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="5"/>
-    </row>
-    <row r="16" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C15" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="K15" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L15" s="10"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="16"/>
+      <c r="R15" s="19"/>
+      <c r="S15" s="20"/>
+      <c r="T15" s="19"/>
+    </row>
+    <row r="16" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>13</v>
       </c>
@@ -757,8 +1397,27 @@
         <v>15</v>
       </c>
       <c r="C16" s="5"/>
-    </row>
-    <row r="17" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D16" s="10"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L16" s="10"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="16"/>
+      <c r="R16" s="19"/>
+      <c r="S16" s="20"/>
+      <c r="T16" s="19"/>
+    </row>
+    <row r="17" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>14</v>
       </c>
@@ -766,8 +1425,27 @@
         <v>16</v>
       </c>
       <c r="C17" s="5"/>
-    </row>
-    <row r="18" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D17" s="10"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L17" s="10"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="19"/>
+      <c r="S17" s="20"/>
+      <c r="T17" s="19"/>
+    </row>
+    <row r="18" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>15</v>
       </c>
@@ -775,8 +1453,27 @@
         <v>17</v>
       </c>
       <c r="C18" s="5"/>
-    </row>
-    <row r="19" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D18" s="10"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L18" s="10"/>
+      <c r="M18" s="16"/>
+      <c r="N18" s="15"/>
+      <c r="O18" s="16"/>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="16"/>
+      <c r="R18" s="19"/>
+      <c r="S18" s="20"/>
+      <c r="T18" s="19"/>
+    </row>
+    <row r="19" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>16</v>
       </c>
@@ -784,8 +1481,27 @@
         <v>18</v>
       </c>
       <c r="C19" s="5"/>
-    </row>
-    <row r="20" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D19" s="10"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L19" s="10"/>
+      <c r="M19" s="16"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="16"/>
+      <c r="P19" s="15"/>
+      <c r="Q19" s="16"/>
+      <c r="R19" s="19"/>
+      <c r="S19" s="20"/>
+      <c r="T19" s="19"/>
+    </row>
+    <row r="20" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <v>17</v>
       </c>
@@ -793,8 +1509,27 @@
         <v>19</v>
       </c>
       <c r="C20" s="5"/>
-    </row>
-    <row r="21" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D20" s="10"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L20" s="10"/>
+      <c r="M20" s="16"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="16"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="16"/>
+      <c r="R20" s="19"/>
+      <c r="S20" s="20"/>
+      <c r="T20" s="19"/>
+    </row>
+    <row r="21" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <v>18</v>
       </c>
@@ -802,17 +1537,57 @@
         <v>20</v>
       </c>
       <c r="C21" s="5"/>
-    </row>
-    <row r="22" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D21" s="10"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L21" s="10"/>
+      <c r="M21" s="16"/>
+      <c r="N21" s="15"/>
+      <c r="O21" s="16"/>
+      <c r="P21" s="15"/>
+      <c r="Q21" s="16"/>
+      <c r="R21" s="19"/>
+      <c r="S21" s="20"/>
+      <c r="T21" s="19"/>
+    </row>
+    <row r="22" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <v>19</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="5"/>
-    </row>
-    <row r="23" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C22" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="10"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L22" s="10"/>
+      <c r="M22" s="16"/>
+      <c r="N22" s="15"/>
+      <c r="O22" s="16"/>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="16"/>
+      <c r="R22" s="19"/>
+      <c r="S22" s="20"/>
+      <c r="T22" s="19"/>
+    </row>
+    <row r="23" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <v>20</v>
       </c>
@@ -820,8 +1595,27 @@
         <v>22</v>
       </c>
       <c r="C23" s="5"/>
-    </row>
-    <row r="24" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D23" s="10"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L23" s="10"/>
+      <c r="M23" s="16"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="16"/>
+      <c r="P23" s="15"/>
+      <c r="Q23" s="16"/>
+      <c r="R23" s="19"/>
+      <c r="S23" s="20"/>
+      <c r="T23" s="19"/>
+    </row>
+    <row r="24" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <v>21</v>
       </c>
@@ -829,8 +1623,27 @@
         <v>23</v>
       </c>
       <c r="C24" s="5"/>
-    </row>
-    <row r="25" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D24" s="10"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L24" s="10"/>
+      <c r="M24" s="16"/>
+      <c r="N24" s="15"/>
+      <c r="O24" s="16"/>
+      <c r="P24" s="15"/>
+      <c r="Q24" s="16"/>
+      <c r="R24" s="19"/>
+      <c r="S24" s="20"/>
+      <c r="T24" s="19"/>
+    </row>
+    <row r="25" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <v>22</v>
       </c>
@@ -838,8 +1651,27 @@
         <v>24</v>
       </c>
       <c r="C25" s="5"/>
-    </row>
-    <row r="26" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D25" s="10"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L25" s="10"/>
+      <c r="M25" s="16"/>
+      <c r="N25" s="15"/>
+      <c r="O25" s="16"/>
+      <c r="P25" s="15"/>
+      <c r="Q25" s="16"/>
+      <c r="R25" s="19"/>
+      <c r="S25" s="20"/>
+      <c r="T25" s="19"/>
+    </row>
+    <row r="26" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <v>23</v>
       </c>
@@ -849,8 +1681,27 @@
       <c r="C26" s="5" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D26" s="10"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L26" s="10"/>
+      <c r="M26" s="16"/>
+      <c r="N26" s="15"/>
+      <c r="O26" s="16"/>
+      <c r="P26" s="15"/>
+      <c r="Q26" s="16"/>
+      <c r="R26" s="19"/>
+      <c r="S26" s="20"/>
+      <c r="T26" s="19"/>
+    </row>
+    <row r="27" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <v>24</v>
       </c>
@@ -858,17 +1709,59 @@
         <v>26</v>
       </c>
       <c r="C27" s="5"/>
-    </row>
-    <row r="28" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D27" s="10"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="K27" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L27" s="10"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="15"/>
+      <c r="O27" s="16"/>
+      <c r="P27" s="15"/>
+      <c r="Q27" s="16"/>
+      <c r="R27" s="19"/>
+      <c r="S27" s="20"/>
+      <c r="T27" s="19"/>
+    </row>
+    <row r="28" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <v>25</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="5"/>
-    </row>
-    <row r="29" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C28" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" s="10"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L28" s="10"/>
+      <c r="M28" s="16"/>
+      <c r="N28" s="15"/>
+      <c r="O28" s="16"/>
+      <c r="P28" s="15"/>
+      <c r="Q28" s="16"/>
+      <c r="R28" s="19"/>
+      <c r="S28" s="20"/>
+      <c r="T28" s="19"/>
+    </row>
+    <row r="29" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <v>26</v>
       </c>
@@ -876,8 +1769,29 @@
         <v>28</v>
       </c>
       <c r="C29" s="5"/>
-    </row>
-    <row r="30" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D29" s="10"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="K29" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L29" s="10"/>
+      <c r="M29" s="16"/>
+      <c r="N29" s="15"/>
+      <c r="O29" s="16"/>
+      <c r="P29" s="15"/>
+      <c r="Q29" s="16"/>
+      <c r="R29" s="19"/>
+      <c r="S29" s="20"/>
+      <c r="T29" s="19"/>
+    </row>
+    <row r="30" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
         <v>27</v>
       </c>
@@ -885,26 +1799,87 @@
         <v>29</v>
       </c>
       <c r="C30" s="5"/>
-    </row>
-    <row r="31" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D30" s="10"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L30" s="10"/>
+      <c r="M30" s="16"/>
+      <c r="N30" s="15"/>
+      <c r="O30" s="16"/>
+      <c r="P30" s="15"/>
+      <c r="Q30" s="16"/>
+      <c r="R30" s="19"/>
+      <c r="S30" s="20"/>
+      <c r="T30" s="19"/>
+    </row>
+    <row r="31" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="6">
         <v>28</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C31" s="5"/>
-    </row>
-    <row r="32" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C31" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D31" s="10"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L31" s="10"/>
+      <c r="M31" s="16"/>
+      <c r="N31" s="15"/>
+      <c r="O31" s="16"/>
+      <c r="P31" s="15"/>
+      <c r="Q31" s="16"/>
+      <c r="R31" s="19"/>
+      <c r="S31" s="20"/>
+      <c r="T31" s="19"/>
+    </row>
+    <row r="32" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="6">
         <v>29</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="5"/>
-    </row>
-    <row r="33" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C32" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D32" s="13"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L32" s="10"/>
+      <c r="M32" s="16"/>
+      <c r="N32" s="15"/>
+      <c r="O32" s="16"/>
+      <c r="P32" s="15"/>
+      <c r="Q32" s="16"/>
+      <c r="R32" s="19"/>
+      <c r="S32" s="20"/>
+      <c r="T32" s="19"/>
+    </row>
+    <row r="33" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="6">
         <v>30</v>
       </c>
@@ -912,8 +1887,27 @@
         <v>32</v>
       </c>
       <c r="C33" s="5"/>
-    </row>
-    <row r="34" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D33" s="10"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L33" s="10"/>
+      <c r="M33" s="16"/>
+      <c r="N33" s="15"/>
+      <c r="O33" s="16"/>
+      <c r="P33" s="15"/>
+      <c r="Q33" s="16"/>
+      <c r="R33" s="19"/>
+      <c r="S33" s="20"/>
+      <c r="T33" s="19"/>
+    </row>
+    <row r="34" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="6">
         <v>31</v>
       </c>
@@ -921,35 +1915,117 @@
         <v>33</v>
       </c>
       <c r="C34" s="5"/>
-    </row>
-    <row r="35" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D34" s="10"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L34" s="10"/>
+      <c r="M34" s="16"/>
+      <c r="N34" s="15"/>
+      <c r="O34" s="16"/>
+      <c r="P34" s="15"/>
+      <c r="Q34" s="16"/>
+      <c r="R34" s="19"/>
+      <c r="S34" s="20"/>
+      <c r="T34" s="19"/>
+    </row>
+    <row r="35" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="6">
         <v>32</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C35" s="5"/>
-    </row>
-    <row r="36" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C35" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D35" s="10"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="10"/>
+      <c r="K35" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L35" s="10"/>
+      <c r="M35" s="16"/>
+      <c r="N35" s="15"/>
+      <c r="O35" s="16"/>
+      <c r="P35" s="15"/>
+      <c r="Q35" s="16"/>
+      <c r="R35" s="19"/>
+      <c r="S35" s="20"/>
+      <c r="T35" s="19"/>
+    </row>
+    <row r="36" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="6">
         <v>33</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="5"/>
-    </row>
-    <row r="37" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C36" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D36" s="10"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L36" s="10"/>
+      <c r="M36" s="16"/>
+      <c r="N36" s="15"/>
+      <c r="O36" s="16"/>
+      <c r="P36" s="15"/>
+      <c r="Q36" s="16"/>
+      <c r="R36" s="19"/>
+      <c r="S36" s="20"/>
+      <c r="T36" s="19"/>
+    </row>
+    <row r="37" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="6">
         <v>34</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C37" s="5"/>
-    </row>
-    <row r="38" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C37" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D37" s="10"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="10"/>
+      <c r="K37" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L37" s="10"/>
+      <c r="M37" s="16"/>
+      <c r="N37" s="15"/>
+      <c r="O37" s="16"/>
+      <c r="P37" s="15"/>
+      <c r="Q37" s="16"/>
+      <c r="R37" s="19"/>
+      <c r="S37" s="20"/>
+      <c r="T37" s="19"/>
+    </row>
+    <row r="38" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="6">
         <v>35</v>
       </c>
@@ -957,17 +2033,41 @@
         <v>37</v>
       </c>
       <c r="C38" s="5"/>
-    </row>
-    <row r="40" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="41" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="42" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="K38" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L38" s="10"/>
+      <c r="M38" s="16"/>
+      <c r="N38" s="15"/>
+      <c r="O38" s="16"/>
+      <c r="P38" s="15"/>
+      <c r="Q38" s="16"/>
+      <c r="R38" s="19"/>
+      <c r="S38" s="20"/>
+      <c r="T38" s="19"/>
+    </row>
+    <row r="40" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B1:B3"/>
+    <mergeCell ref="D1:L1"/>
+    <mergeCell ref="M1:Q1"/>
+    <mergeCell ref="R1:T1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B4:B38">

</xml_diff>